<commit_message>
update the files to match the lastest AgMIP protocol
</commit_message>
<xml_diff>
--- a/Maize_Machakos/raw/Field_Overlay-Machakos-MAZ.xlsx
+++ b/Maize_Machakos/raw/Field_Overlay-Machakos-MAZ.xlsx
@@ -1188,11 +1188,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N163"/>
+  <dimension ref="A1:N165"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
@@ -3526,6 +3524,9 @@
       <c r="F163">
         <v>200</v>
       </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="D165"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>